<commit_message>
Still putting the pieces together
</commit_message>
<xml_diff>
--- a/charts_xlsx/rbchart.xlsx
+++ b/charts_xlsx/rbchart.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2015" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1991" uniqueCount="424">
   <si>
     <t>Sign Degree: [Planet]</t>
   </si>
@@ -613,22 +613,19 @@
     <t xml:space="preserve">64: [-4 SEPARATING TRINE to SUN; -3 SEPARATING TRINE to VENUS; 3 APPLYING OPPOSITION to SATURN] </t>
   </si>
   <si>
-    <t>Diamonds, Triangles, or Leaves 
+    <t>64: [Diamonds, Triangles, or Leaves 
  Exactness Stitch Width: 6 
  Aspect K/P:PatternStitchBase.PURL 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3]</t>
-  </si>
-  <si>
-    <t>Diamonds, Triangles, or Leaves 
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
+ Tot Dig Score: 5; Diamonds, Triangles, or Leaves 
  Exactness Stitch Width: 7 
  Aspect K/P:PatternStitchBase.PURL 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3]</t>
-  </si>
-  <si>
-    <t>Circles, Chains, or Honeycomb 
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
+ Tot Dig Score: 1; Circles, Chains, or Honeycomb 
  Exactness Stitch Width: 7 
  Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3]</t>
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
+ Tot Dig Score: 1]</t>
   </si>
   <si>
     <t>66</t>
@@ -769,28 +766,23 @@
     <t xml:space="preserve">131: [-10 APPLYING OPPOSITION to VENUS; -4 APPLYING TRINE to SATURN; -1 APPLYING BIQUINTILE to NEPTUNE; -4 APPLYING SQUARE to PLUTO] </t>
   </si>
   <si>
-    <t>Circles, Chains, or Honeycomb 
+    <t>131: [Circles, Chains, or Honeycomb 
  Exactness Stitch Width: 0 
  Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3]</t>
-  </si>
-  <si>
-    <t>Diamonds, Triangles, or Leaves 
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
+ Tot Dig Score: 0; Diamonds, Triangles, or Leaves 
  Exactness Stitch Width: 6 
  Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
+ Tot Dig Score: 0;  
  Exactness Stitch Width: 9 
  Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3]</t>
-  </si>
-  <si>
-    <t>Squares, or Diamonds 
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
+ Tot Dig Score: 0; Squares, or Diamonds 
  Exactness Stitch Width: 6 
  Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3]</t>
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
+ Tot Dig Score: 0]</t>
   </si>
   <si>
     <t>132</t>
@@ -973,28 +965,27 @@
     <t xml:space="preserve">217: [-7 APPLYING SQUARE to SUN; -4 APPLYING SQUARE to ASC; -6 APPLYING SQUARE to VENUS; -2 APPLYING SEMISQUARE to URANUS; -3 APPLYING SEXTILE to NEPTUNE] </t>
   </si>
   <si>
-    <t>Squares, or Diamonds 
+    <t>217: [Squares, or Diamonds 
  Exactness Stitch Width: 3 
  Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3]</t>
-  </si>
-  <si>
-    <t>Squares, or Diamonds 
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
+ Tot Dig Score: 4; Squares, or Diamonds 
+ Exactness Stitch Width: 6 
+ Aspect K/P:PatternStitchBase.KNIT 
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
+ Tot Dig Score: 0; Squares, or Diamonds 
  Exactness Stitch Width: 4 
  Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3]</t>
-  </si>
-  <si>
-    <t>Chevron 
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
+ Tot Dig Score: 0; Chevron 
  Exactness Stitch Width: 8 
  Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3]</t>
-  </si>
-  <si>
-    <t>Stars, Snowflake, or Leaves 
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
+ Tot Dig Score: 0; Stars, Snowflake, or Leaves 
  Exactness Stitch Width: 7 
  Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3]</t>
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
+ Tot Dig Score: 0]</t>
   </si>
   <si>
     <t>219</t>
@@ -1033,16 +1024,15 @@
     <t xml:space="preserve">232: [1 SEPARATING SEXTILE to MERCURY; -2 SEPARATING SEMISEXTILE to URANUS] </t>
   </si>
   <si>
-    <t>Stars, Snowflake, or Leaves 
+    <t>232: [Stars, Snowflake, or Leaves 
  Exactness Stitch Width: 9 
  Aspect K/P:PatternStitchBase.PURL 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3]</t>
-  </si>
-  <si>
-    <t>Snowflake 
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
+ Tot Dig Score: 0; Snowflake 
  Exactness Stitch Width: 8 
  Aspect K/P:PatternStitchBase.PURL 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3]</t>
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
+ Tot Dig Score: 0]</t>
   </si>
   <si>
     <t>234</t>
@@ -1081,16 +1071,23 @@
     <t xml:space="preserve">247: [3 APPLYING OPPOSITION to MOON; -4 APPLYING TRINE to ASC; 1 SEPARATING SEMISQUARE to MERCURY; -6 APPLYING SEXTILE to VENUS] </t>
   </si>
   <si>
-    <t>Chevron 
+    <t>247: [Circles, Chains, or Honeycomb 
+ Exactness Stitch Width: 7 
+ Aspect K/P:PatternStitchBase.KNIT 
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
+ Tot Dig Score: 1; Diamonds, Triangles, or Leaves 
+ Exactness Stitch Width: 6 
+ Aspect K/P:PatternStitchBase.KNIT 
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
+ Tot Dig Score: 0; Chevron 
  Exactness Stitch Width: 9 
  Aspect K/P:PatternStitchBase.PURL 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3]</t>
-  </si>
-  <si>
-    <t>Stars, Snowflake, or Leaves 
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
+ Tot Dig Score: 0; Stars, Snowflake, or Leaves 
  Exactness Stitch Width: 4 
  Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3]</t>
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
+ Tot Dig Score: 0]</t>
   </si>
   <si>
     <t>249</t>
@@ -1123,10 +1120,19 @@
     <t xml:space="preserve">260: [-2 SEPARATING SEMISEXTILE to MARS; 2 SEPARATING SEXTILE to JUPITER; -2 APPLYING SEMISQUARE to PLUTO] </t>
   </si>
   <si>
-    <t>Stars, Snowflake, or Leaves 
+    <t>260: [Snowflake 
  Exactness Stitch Width: 8 
  Aspect K/P:PatternStitchBase.PURL 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3]</t>
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
+ Tot Dig Score: 0; Stars, Snowflake, or Leaves 
+ Exactness Stitch Width: 8 
+ Aspect K/P:PatternStitchBase.PURL 
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
+ Tot Dig Score: 0; Chevron 
+ Exactness Stitch Width: 8 
+ Aspect K/P:PatternStitchBase.KNIT 
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
+ Tot Dig Score: 0]</t>
   </si>
   <si>
     <t>261</t>
@@ -1165,6 +1171,17 @@
     <t xml:space="preserve">274: [-1 APPLYING BIQUINTILE to ASC; -3 APPLYING SEXTILE to PLUTO] </t>
   </si>
   <si>
+    <t>274: [ 
+ Exactness Stitch Width: 9 
+ Aspect K/P:PatternStitchBase.KNIT 
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
+ Tot Dig Score: 0; Stars, Snowflake, or Leaves 
+ Exactness Stitch Width: 7 
+ Aspect K/P:PatternStitchBase.KNIT 
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
+ Tot Dig Score: 0]</t>
+  </si>
+  <si>
     <t>276</t>
   </si>
   <si>
@@ -1207,55 +1224,73 @@
     <t xml:space="preserve">293: [7 APPLYING CONJ to SUN; 8 APPLYING CONJ to VENUS; 1 SEPARATING SEXTILE to MARS; -1 SEPARATING SEMISEXTILE to JUPITER; 1 SEPARATING SEMISQUARE to SATURN] </t>
   </si>
   <si>
-    <t>Lines, circles, or Chains 
+    <t>293: [Lines, circles, or Chains 
  Exactness Stitch Width: 3 
  Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3]</t>
-  </si>
-  <si>
-    <t>Lines, circles, or Chains 
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
+ Tot Dig Score: 4; Lines, circles, or Chains 
  Exactness Stitch Width: 2 
  Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3]</t>
-  </si>
-  <si>
-    <t>Snowflake 
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
+ Tot Dig Score: 0; Stars, Snowflake, or Leaves 
  Exactness Stitch Width: 9 
  Aspect K/P:PatternStitchBase.PURL 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3]</t>
-  </si>
-  <si>
-    <t>294</t>
-  </si>
-  <si>
-    <t>24 Capricorn</t>
-  </si>
-  <si>
-    <t>297</t>
-  </si>
-  <si>
-    <t>27 Capricorn</t>
-  </si>
-  <si>
-    <t>300</t>
-  </si>
-  <si>
-    <t>0 Aquarius</t>
-  </si>
-  <si>
-    <t xml:space="preserve">300: [SUN] </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DETRIMENT: [4] </t>
-  </si>
-  <si>
-    <t xml:space="preserve">300: [-4 SEPARATING TRINE to MOON; 7 APPLYING CONJ to MERCURY; 1 SEPARATING CONJ to VENUS; -7 APPLYING SQUARE to PLUTO] </t>
-  </si>
-  <si>
-    <t>Lines, circles, or Chains 
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
+ Tot Dig Score: 0; Snowflake 
  Exactness Stitch Width: 9 
  Aspect K/P:PatternStitchBase.PURL 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3]</t>
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
+ Tot Dig Score: 0; Chevron 
+ Exactness Stitch Width: 9 
+ Aspect K/P:PatternStitchBase.PURL 
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
+ Tot Dig Score: 0]</t>
+  </si>
+  <si>
+    <t>294</t>
+  </si>
+  <si>
+    <t>24 Capricorn</t>
+  </si>
+  <si>
+    <t>297</t>
+  </si>
+  <si>
+    <t>27 Capricorn</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t>0 Aquarius</t>
+  </si>
+  <si>
+    <t xml:space="preserve">300: [SUN] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DETRIMENT: [4] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">300: [-4 SEPARATING TRINE to MOON; 7 APPLYING CONJ to MERCURY; 1 SEPARATING CONJ to VENUS; -7 APPLYING SQUARE to PLUTO] </t>
+  </si>
+  <si>
+    <t>300: [Diamonds, Triangles, or Leaves 
+ Exactness Stitch Width: 6 
+ Aspect K/P:PatternStitchBase.PURL 
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
+ Tot Dig Score: 5; Lines, circles, or Chains 
+ Exactness Stitch Width: 3 
+ Aspect K/P:PatternStitchBase.KNIT 
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
+ Tot Dig Score: 4; Lines, circles, or Chains 
+ Exactness Stitch Width: 9 
+ Aspect K/P:PatternStitchBase.PURL 
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
+ Tot Dig Score: 4; Squares, or Diamonds 
+ Exactness Stitch Width: 3 
+ Aspect K/P:PatternStitchBase.KNIT 
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
+ Tot Dig Score: 4]</t>
   </si>
   <si>
     <t>303</t>
@@ -1304,6 +1339,17 @@
   </si>
   <si>
     <t xml:space="preserve">322: [-1 SEPARATING SEMISEXTILE to MERCURY; 2 SEPARATING SEXTILE to URANUS] </t>
+  </si>
+  <si>
+    <t>322: [Snowflake 
+ Exactness Stitch Width: 9 
+ Aspect K/P:PatternStitchBase.PURL 
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
+ Tot Dig Score: 0; Stars, Snowflake, or Leaves 
+ Exactness Stitch Width: 8 
+ Aspect K/P:PatternStitchBase.PURL 
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
+ Tot Dig Score: 0]</t>
   </si>
   <si>
     <t>324</t>
@@ -2595,7 +2641,7 @@
         <v>155</v>
       </c>
       <c r="AF23" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="AG23">
         <v>22</v>
@@ -2603,10 +2649,10 @@
     </row>
     <row r="24" spans="2:33">
       <c r="E24" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F24" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>53</v>
@@ -2632,10 +2678,10 @@
     </row>
     <row r="25" spans="2:33">
       <c r="E25" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F25" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>57</v>
@@ -2655,10 +2701,10 @@
     </row>
     <row r="26" spans="2:33">
       <c r="E26" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F26" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>57</v>
@@ -2681,10 +2727,10 @@
     </row>
     <row r="27" spans="2:33">
       <c r="E27" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F27" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I27" s="8" t="s">
         <v>69</v>
@@ -2707,10 +2753,10 @@
     </row>
     <row r="28" spans="2:33">
       <c r="E28" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F28" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L28" s="12" t="s">
         <v>105</v>
@@ -2727,10 +2773,10 @@
     </row>
     <row r="29" spans="2:33">
       <c r="E29" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F29" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>54</v>
@@ -2753,10 +2799,10 @@
     </row>
     <row r="30" spans="2:33">
       <c r="E30" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F30" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>54</v>
@@ -2782,10 +2828,10 @@
     </row>
     <row r="31" spans="2:33">
       <c r="E31" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F31" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>55</v>
@@ -2811,10 +2857,10 @@
     </row>
     <row r="32" spans="2:33">
       <c r="E32" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>55</v>
@@ -2837,10 +2883,10 @@
     </row>
     <row r="33" spans="2:33">
       <c r="E33" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F33" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>58</v>
@@ -2860,10 +2906,10 @@
     </row>
     <row r="34" spans="2:33">
       <c r="E34" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F34" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="N34" s="5" t="s">
         <v>125</v>
@@ -2880,10 +2926,10 @@
     </row>
     <row r="35" spans="2:33">
       <c r="E35" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F35" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I35" s="8" t="s">
         <v>68</v>
@@ -2900,10 +2946,10 @@
     </row>
     <row r="36" spans="2:33">
       <c r="E36" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F36" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I36" s="8" t="s">
         <v>68</v>
@@ -2926,10 +2972,10 @@
     </row>
     <row r="37" spans="2:33">
       <c r="E37" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F37" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>60</v>
@@ -2949,10 +2995,10 @@
     </row>
     <row r="38" spans="2:33">
       <c r="E38" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F38" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>56</v>
@@ -2978,10 +3024,10 @@
     </row>
     <row r="39" spans="2:33">
       <c r="E39" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F39" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>56</v>
@@ -3007,10 +3053,10 @@
     </row>
     <row r="40" spans="2:33">
       <c r="E40" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F40" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>56</v>
@@ -3030,10 +3076,10 @@
     </row>
     <row r="41" spans="2:33">
       <c r="E41" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F41" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>56</v>
@@ -3062,10 +3108,10 @@
     </row>
     <row r="42" spans="2:33">
       <c r="E42" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F42" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>56</v>
@@ -3097,10 +3143,10 @@
     </row>
     <row r="43" spans="2:33">
       <c r="E43" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F43" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>56</v>
@@ -3129,10 +3175,10 @@
     </row>
     <row r="44" spans="2:33">
       <c r="E44" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F44" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>56</v>
@@ -3158,16 +3204,16 @@
     </row>
     <row r="45" spans="2:33">
       <c r="B45" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D45" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E45" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F45" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>56</v>
@@ -3188,7 +3234,7 @@
         <v>152</v>
       </c>
       <c r="AF45" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="AG45">
         <v>44</v>
@@ -3196,10 +3242,10 @@
     </row>
     <row r="46" spans="2:33">
       <c r="E46" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="F46" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="I46" s="8" t="s">
         <v>67</v>
@@ -3225,10 +3271,10 @@
     </row>
     <row r="47" spans="2:33">
       <c r="E47" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="F47" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="H47" s="3" t="s">
         <v>61</v>
@@ -3251,10 +3297,10 @@
     </row>
     <row r="48" spans="2:33">
       <c r="E48" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="F48" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="I48" s="8" t="s">
         <v>67</v>
@@ -3274,10 +3320,10 @@
     </row>
     <row r="49" spans="5:33">
       <c r="E49" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="F49" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="J49" s="9" t="s">
         <v>85</v>
@@ -3297,10 +3343,10 @@
     </row>
     <row r="50" spans="5:33">
       <c r="E50" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="F50" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="H50" s="3" t="s">
         <v>62</v>
@@ -3326,10 +3372,10 @@
     </row>
     <row r="51" spans="5:33">
       <c r="E51" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="F51" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>55</v>
@@ -3361,10 +3407,10 @@
     </row>
     <row r="52" spans="5:33">
       <c r="E52" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="F52" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>55</v>
@@ -3393,10 +3439,10 @@
     </row>
     <row r="53" spans="5:33">
       <c r="E53" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="F53" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="H53" s="3" t="s">
         <v>62</v>
@@ -3416,10 +3462,10 @@
     </row>
     <row r="54" spans="5:33">
       <c r="E54" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="F54" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="H54" s="3" t="s">
         <v>62</v>
@@ -3439,10 +3485,10 @@
     </row>
     <row r="55" spans="5:33">
       <c r="E55" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="F55" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="H55" s="3" t="s">
         <v>62</v>
@@ -3465,10 +3511,10 @@
     </row>
     <row r="56" spans="5:33">
       <c r="E56" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="F56" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="I56" s="8" t="s">
         <v>68</v>
@@ -3488,10 +3534,10 @@
     </row>
     <row r="57" spans="5:33">
       <c r="E57" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="F57" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="J57" s="9" t="s">
         <v>83</v>
@@ -3508,10 +3554,10 @@
     </row>
     <row r="58" spans="5:33">
       <c r="E58" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="F58" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="J58" s="9" t="s">
         <v>83</v>
@@ -3531,10 +3577,10 @@
     </row>
     <row r="59" spans="5:33">
       <c r="E59" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="F59" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>53</v>
@@ -3560,10 +3606,10 @@
     </row>
     <row r="60" spans="5:33">
       <c r="E60" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="F60" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>53</v>
@@ -3595,10 +3641,10 @@
     </row>
     <row r="61" spans="5:33">
       <c r="E61" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="F61" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>53</v>
@@ -3630,10 +3676,10 @@
     </row>
     <row r="62" spans="5:33">
       <c r="E62" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="F62" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>53</v>
@@ -3659,10 +3705,10 @@
     </row>
     <row r="63" spans="5:33">
       <c r="E63" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="F63" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>53</v>
@@ -3691,10 +3737,10 @@
     </row>
     <row r="64" spans="5:33">
       <c r="E64" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="F64" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>53</v>
@@ -3723,10 +3769,10 @@
     </row>
     <row r="65" spans="2:33">
       <c r="E65" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="F65" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="H65" s="3" t="s">
         <v>63</v>
@@ -3746,10 +3792,10 @@
     </row>
     <row r="66" spans="2:33">
       <c r="E66" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="F66" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="I66" s="8" t="s">
         <v>69</v>
@@ -3769,10 +3815,10 @@
     </row>
     <row r="67" spans="2:33">
       <c r="E67" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="F67" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="I67" s="8" t="s">
         <v>69</v>
@@ -3792,10 +3838,10 @@
     </row>
     <row r="68" spans="2:33">
       <c r="E68" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="F68" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="J68" s="9" t="s">
         <v>82</v>
@@ -3815,10 +3861,10 @@
     </row>
     <row r="69" spans="2:33">
       <c r="E69" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="F69" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>52</v>
@@ -3847,10 +3893,10 @@
     </row>
     <row r="70" spans="2:33">
       <c r="E70" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="F70" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>52</v>
@@ -3873,10 +3919,10 @@
     </row>
     <row r="71" spans="2:33">
       <c r="E71" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="F71" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>52</v>
@@ -3905,10 +3951,10 @@
     </row>
     <row r="72" spans="2:33">
       <c r="E72" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="F72" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>52</v>
@@ -3934,10 +3980,10 @@
     </row>
     <row r="73" spans="2:33">
       <c r="E73" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="F73" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="G73" s="2" t="s">
         <v>52</v>
@@ -3966,16 +4012,16 @@
     </row>
     <row r="74" spans="2:33">
       <c r="B74" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="D74" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="E74" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="F74" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="G74" s="2" t="s">
         <v>52</v>
@@ -3996,7 +4042,7 @@
         <v>147</v>
       </c>
       <c r="AF74" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="AG74">
         <v>73</v>
@@ -4004,10 +4050,10 @@
     </row>
     <row r="75" spans="2:33">
       <c r="E75" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="F75" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="I75" s="8" t="s">
         <v>72</v>
@@ -4024,10 +4070,10 @@
     </row>
     <row r="76" spans="2:33">
       <c r="E76" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="F76" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="I76" s="8" t="s">
         <v>72</v>
@@ -4047,10 +4093,10 @@
     </row>
     <row r="77" spans="2:33">
       <c r="E77" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="F77" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="I77" s="8" t="s">
         <v>72</v>
@@ -4073,10 +4119,10 @@
     </row>
     <row r="78" spans="2:33">
       <c r="E78" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="F78" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="I78" s="8" t="s">
         <v>72</v>
@@ -4099,16 +4145,16 @@
     </row>
     <row r="79" spans="2:33">
       <c r="B79" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="D79" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="E79" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="F79" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="J79" s="9" t="s">
         <v>79</v>
@@ -4123,7 +4169,7 @@
         <v>128</v>
       </c>
       <c r="AF79" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="AG79">
         <v>78</v>
@@ -4131,10 +4177,10 @@
     </row>
     <row r="80" spans="2:33">
       <c r="E80" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="F80" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="G80" s="2" t="s">
         <v>49</v>
@@ -4160,10 +4206,10 @@
     </row>
     <row r="81" spans="2:33">
       <c r="E81" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="F81" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="G81" s="2" t="s">
         <v>49</v>
@@ -4192,10 +4238,10 @@
     </row>
     <row r="82" spans="2:33">
       <c r="E82" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="F82" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="G82" s="2" t="s">
         <v>49</v>
@@ -4221,10 +4267,10 @@
     </row>
     <row r="83" spans="2:33">
       <c r="E83" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="F83" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>49</v>
@@ -4253,16 +4299,16 @@
     </row>
     <row r="84" spans="2:33">
       <c r="B84" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="D84" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="E84" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="F84" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="H84" s="3" t="s">
         <v>66</v>
@@ -4280,7 +4326,7 @@
         <v>148</v>
       </c>
       <c r="AF84" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="AG84">
         <v>83</v>
@@ -4288,10 +4334,10 @@
     </row>
     <row r="85" spans="2:33">
       <c r="E85" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="F85" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="H85" s="3" t="s">
         <v>66</v>
@@ -4311,10 +4357,10 @@
     </row>
     <row r="86" spans="2:33">
       <c r="E86" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="F86" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="H86" s="3" t="s">
         <v>66</v>
@@ -4334,10 +4380,10 @@
     </row>
     <row r="87" spans="2:33">
       <c r="E87" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="F87" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="I87" s="8" t="s">
         <v>73</v>
@@ -4357,16 +4403,16 @@
     </row>
     <row r="88" spans="2:33">
       <c r="B88" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="D88" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="E88" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="F88" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="I88" s="8" t="s">
         <v>73</v>
@@ -4384,7 +4430,7 @@
         <v>150</v>
       </c>
       <c r="AF88" t="s">
-        <v>314</v>
+        <v>344</v>
       </c>
       <c r="AG88">
         <v>87</v>
@@ -4392,10 +4438,10 @@
     </row>
     <row r="89" spans="2:33">
       <c r="E89" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="F89" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="J89" s="9" t="s">
         <v>78</v>
@@ -4418,10 +4464,10 @@
     </row>
     <row r="90" spans="2:33">
       <c r="E90" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="F90" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="J90" s="9" t="s">
         <v>78</v>
@@ -4441,10 +4487,10 @@
     </row>
     <row r="91" spans="2:33">
       <c r="E91" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="F91" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="G91" s="2" t="s">
         <v>48</v>
@@ -4467,10 +4513,10 @@
     </row>
     <row r="92" spans="2:33">
       <c r="E92" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="F92" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="G92" s="2" t="s">
         <v>48</v>
@@ -4493,16 +4539,16 @@
     </row>
     <row r="93" spans="2:33">
       <c r="B93" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="D93" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="E93" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="F93" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="H93" s="3" t="s">
         <v>65</v>
@@ -4523,7 +4569,7 @@
         <v>149</v>
       </c>
       <c r="AF93" t="s">
-        <v>315</v>
+        <v>357</v>
       </c>
       <c r="AG93">
         <v>92</v>
@@ -4531,10 +4577,10 @@
     </row>
     <row r="94" spans="2:33">
       <c r="E94" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="F94" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="L94" s="12" t="s">
         <v>100</v>
@@ -4554,10 +4600,10 @@
     </row>
     <row r="95" spans="2:33">
       <c r="E95" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="F95" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="I95" s="8" t="s">
         <v>75</v>
@@ -4574,10 +4620,10 @@
     </row>
     <row r="96" spans="2:33">
       <c r="E96" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="F96" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="I96" s="8" t="s">
         <v>75</v>
@@ -4597,10 +4643,10 @@
     </row>
     <row r="97" spans="2:33">
       <c r="E97" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
       <c r="F97" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="J97" s="9" t="s">
         <v>77</v>
@@ -4614,10 +4660,10 @@
     </row>
     <row r="98" spans="2:33">
       <c r="E98" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="F98" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="G98" s="2" t="s">
         <v>47</v>
@@ -4646,16 +4692,16 @@
     </row>
     <row r="99" spans="2:33">
       <c r="B99" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="D99" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
       <c r="E99" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="F99" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="G99" s="2" t="s">
         <v>47</v>
@@ -4679,7 +4725,7 @@
         <v>128</v>
       </c>
       <c r="AF99" t="s">
-        <v>342</v>
+        <v>372</v>
       </c>
       <c r="AG99">
         <v>98</v>
@@ -4687,10 +4733,10 @@
     </row>
     <row r="100" spans="2:33">
       <c r="E100" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
       <c r="F100" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
       <c r="G100" s="2" t="s">
         <v>47</v>
@@ -4713,10 +4759,10 @@
     </row>
     <row r="101" spans="2:33">
       <c r="E101" t="s">
-        <v>387</v>
+        <v>376</v>
       </c>
       <c r="F101" t="s">
-        <v>386</v>
+        <v>375</v>
       </c>
       <c r="G101" s="2" t="s">
         <v>47</v>
@@ -4742,19 +4788,19 @@
     </row>
     <row r="102" spans="2:33">
       <c r="B102" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="C102" t="s">
-        <v>391</v>
+        <v>380</v>
       </c>
       <c r="D102" t="s">
-        <v>392</v>
+        <v>381</v>
       </c>
       <c r="E102" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="F102" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
       <c r="G102" s="2" t="s">
         <v>47</v>
@@ -4781,7 +4827,7 @@
         <v>152</v>
       </c>
       <c r="AF102" t="s">
-        <v>312</v>
+        <v>382</v>
       </c>
       <c r="AG102">
         <v>101</v>
@@ -4789,10 +4835,10 @@
     </row>
     <row r="103" spans="2:33">
       <c r="E103" t="s">
-        <v>395</v>
+        <v>384</v>
       </c>
       <c r="F103" t="s">
-        <v>394</v>
+        <v>383</v>
       </c>
       <c r="G103" s="2" t="s">
         <v>47</v>
@@ -4827,10 +4873,10 @@
     </row>
     <row r="104" spans="2:33">
       <c r="E104" t="s">
-        <v>397</v>
+        <v>386</v>
       </c>
       <c r="F104" t="s">
-        <v>396</v>
+        <v>385</v>
       </c>
       <c r="G104" s="2" t="s">
         <v>47</v>
@@ -4859,10 +4905,10 @@
     </row>
     <row r="105" spans="2:33">
       <c r="E105" t="s">
-        <v>399</v>
+        <v>388</v>
       </c>
       <c r="F105" t="s">
-        <v>398</v>
+        <v>387</v>
       </c>
       <c r="G105" s="2" t="s">
         <v>47</v>
@@ -4888,10 +4934,10 @@
     </row>
     <row r="106" spans="2:33">
       <c r="E106" t="s">
-        <v>401</v>
+        <v>390</v>
       </c>
       <c r="F106" t="s">
-        <v>400</v>
+        <v>389</v>
       </c>
       <c r="I106" s="8" t="s">
         <v>76</v>
@@ -4917,10 +4963,10 @@
     </row>
     <row r="107" spans="2:33">
       <c r="E107" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
       <c r="F107" t="s">
-        <v>402</v>
+        <v>391</v>
       </c>
       <c r="I107" s="8" t="s">
         <v>76</v>
@@ -4943,10 +4989,10 @@
     </row>
     <row r="108" spans="2:33">
       <c r="E108" t="s">
-        <v>405</v>
+        <v>394</v>
       </c>
       <c r="F108" t="s">
-        <v>404</v>
+        <v>393</v>
       </c>
       <c r="I108" s="8" t="s">
         <v>76</v>
@@ -4972,16 +5018,16 @@
     </row>
     <row r="109" spans="2:33">
       <c r="B109" t="s">
-        <v>408</v>
+        <v>397</v>
       </c>
       <c r="D109" t="s">
-        <v>409</v>
+        <v>398</v>
       </c>
       <c r="E109" t="s">
-        <v>407</v>
+        <v>396</v>
       </c>
       <c r="F109" t="s">
-        <v>406</v>
+        <v>395</v>
       </c>
       <c r="J109" s="9" t="s">
         <v>78</v>
@@ -4996,7 +5042,7 @@
         <v>129</v>
       </c>
       <c r="AF109" t="s">
-        <v>354</v>
+        <v>399</v>
       </c>
       <c r="AG109">
         <v>108</v>
@@ -5004,10 +5050,10 @@
     </row>
     <row r="110" spans="2:33">
       <c r="E110" t="s">
-        <v>411</v>
+        <v>401</v>
       </c>
       <c r="F110" t="s">
-        <v>410</v>
+        <v>400</v>
       </c>
       <c r="H110" s="3" t="s">
         <v>62</v>
@@ -5030,10 +5076,10 @@
     </row>
     <row r="111" spans="2:33">
       <c r="E111" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="F111" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="G111" s="2" t="s">
         <v>48</v>
@@ -5065,10 +5111,10 @@
     </row>
     <row r="112" spans="2:33">
       <c r="E112" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="F112" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
       <c r="G112" s="2" t="s">
         <v>48</v>
@@ -5100,10 +5146,10 @@
     </row>
     <row r="113" spans="5:33">
       <c r="E113" t="s">
-        <v>417</v>
+        <v>407</v>
       </c>
       <c r="F113" t="s">
-        <v>416</v>
+        <v>406</v>
       </c>
       <c r="H113" s="3" t="s">
         <v>62</v>
@@ -5123,10 +5169,10 @@
     </row>
     <row r="114" spans="5:33">
       <c r="E114" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
       <c r="F114" t="s">
-        <v>418</v>
+        <v>408</v>
       </c>
       <c r="H114" s="3" t="s">
         <v>62</v>
@@ -5149,10 +5195,10 @@
     </row>
     <row r="115" spans="5:33">
       <c r="E115" t="s">
-        <v>421</v>
+        <v>411</v>
       </c>
       <c r="F115" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
       <c r="H115" s="3" t="s">
         <v>62</v>
@@ -5178,10 +5224,10 @@
     </row>
     <row r="116" spans="5:33">
       <c r="E116" t="s">
-        <v>423</v>
+        <v>413</v>
       </c>
       <c r="F116" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
       <c r="G116" s="2" t="s">
         <v>50</v>
@@ -5210,10 +5256,10 @@
     </row>
     <row r="117" spans="5:33">
       <c r="E117" t="s">
-        <v>425</v>
+        <v>415</v>
       </c>
       <c r="F117" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="G117" s="2" t="s">
         <v>50</v>
@@ -5239,10 +5285,10 @@
     </row>
     <row r="118" spans="5:33">
       <c r="E118" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="F118" t="s">
-        <v>426</v>
+        <v>416</v>
       </c>
       <c r="J118" s="9" t="s">
         <v>79</v>
@@ -5262,10 +5308,10 @@
     </row>
     <row r="119" spans="5:33">
       <c r="E119" t="s">
-        <v>429</v>
+        <v>419</v>
       </c>
       <c r="F119" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
       <c r="J119" s="9" t="s">
         <v>79</v>
@@ -5285,10 +5331,10 @@
     </row>
     <row r="120" spans="5:33">
       <c r="E120" t="s">
-        <v>431</v>
+        <v>421</v>
       </c>
       <c r="F120" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="G120" s="2" t="s">
         <v>49</v>
@@ -5314,10 +5360,10 @@
     </row>
     <row r="121" spans="5:33">
       <c r="E121" t="s">
-        <v>433</v>
+        <v>423</v>
       </c>
       <c r="F121" t="s">
-        <v>432</v>
+        <v>422</v>
       </c>
       <c r="G121" s="2" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
Fixing up some planet stuff
</commit_message>
<xml_diff>
--- a/charts_xlsx/rbchart.xlsx
+++ b/charts_xlsx/rbchart.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1991" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1983" uniqueCount="416">
   <si>
     <t>Sign Degree: [Planet]</t>
   </si>
@@ -613,19 +613,12 @@
     <t xml:space="preserve">64: [-4 SEPARATING TRINE to SUN; -3 SEPARATING TRINE to VENUS; 3 APPLYING OPPOSITION to SATURN] </t>
   </si>
   <si>
-    <t>64: [Diamonds, Triangles, or Leaves 
+    <t>64: [STITCH DETERMINER FOR: SEPARATING TRINE (MOON, SUN) [Score:Intensity: TRINE:8, Exactness:-4, Collective Planet Speed:17] 
+Diamonds, Triangles, or Leaves 
  Exactness Stitch Width: 6 
  Aspect K/P:PatternStitchBase.PURL 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
- Tot Dig Score: 5; Diamonds, Triangles, or Leaves 
- Exactness Stitch Width: 7 
- Aspect K/P:PatternStitchBase.PURL 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
- Tot Dig Score: 1; Circles, Chains, or Honeycomb 
- Exactness Stitch Width: 7 
- Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
- Tot Dig Score: 1]</t>
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [7, 10] 
+ Tot Dig Score: 5]</t>
   </si>
   <si>
     <t>66</t>
@@ -766,25 +759,6 @@
     <t xml:space="preserve">131: [-10 APPLYING OPPOSITION to VENUS; -4 APPLYING TRINE to SATURN; -1 APPLYING BIQUINTILE to NEPTUNE; -4 APPLYING SQUARE to PLUTO] </t>
   </si>
   <si>
-    <t>131: [Circles, Chains, or Honeycomb 
- Exactness Stitch Width: 0 
- Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
- Tot Dig Score: 0; Diamonds, Triangles, or Leaves 
- Exactness Stitch Width: 6 
- Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
- Tot Dig Score: 0;  
- Exactness Stitch Width: 9 
- Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
- Tot Dig Score: 0; Squares, or Diamonds 
- Exactness Stitch Width: 6 
- Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
- Tot Dig Score: 0]</t>
-  </si>
-  <si>
     <t>132</t>
   </si>
   <si>
@@ -965,29 +939,6 @@
     <t xml:space="preserve">217: [-7 APPLYING SQUARE to SUN; -4 APPLYING SQUARE to ASC; -6 APPLYING SQUARE to VENUS; -2 APPLYING SEMISQUARE to URANUS; -3 APPLYING SEXTILE to NEPTUNE] </t>
   </si>
   <si>
-    <t>217: [Squares, or Diamonds 
- Exactness Stitch Width: 3 
- Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
- Tot Dig Score: 4; Squares, or Diamonds 
- Exactness Stitch Width: 6 
- Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
- Tot Dig Score: 0; Squares, or Diamonds 
- Exactness Stitch Width: 4 
- Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
- Tot Dig Score: 0; Chevron 
- Exactness Stitch Width: 8 
- Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
- Tot Dig Score: 0; Stars, Snowflake, or Leaves 
- Exactness Stitch Width: 7 
- Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
- Tot Dig Score: 0]</t>
-  </si>
-  <si>
     <t>219</t>
   </si>
   <si>
@@ -1024,17 +975,6 @@
     <t xml:space="preserve">232: [1 SEPARATING SEXTILE to MERCURY; -2 SEPARATING SEMISEXTILE to URANUS] </t>
   </si>
   <si>
-    <t>232: [Stars, Snowflake, or Leaves 
- Exactness Stitch Width: 9 
- Aspect K/P:PatternStitchBase.PURL 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
- Tot Dig Score: 0; Snowflake 
- Exactness Stitch Width: 8 
- Aspect K/P:PatternStitchBase.PURL 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
- Tot Dig Score: 0]</t>
-  </si>
-  <si>
     <t>234</t>
   </si>
   <si>
@@ -1071,25 +1011,6 @@
     <t xml:space="preserve">247: [3 APPLYING OPPOSITION to MOON; -4 APPLYING TRINE to ASC; 1 SEPARATING SEMISQUARE to MERCURY; -6 APPLYING SEXTILE to VENUS] </t>
   </si>
   <si>
-    <t>247: [Circles, Chains, or Honeycomb 
- Exactness Stitch Width: 7 
- Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
- Tot Dig Score: 1; Diamonds, Triangles, or Leaves 
- Exactness Stitch Width: 6 
- Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
- Tot Dig Score: 0; Chevron 
- Exactness Stitch Width: 9 
- Aspect K/P:PatternStitchBase.PURL 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
- Tot Dig Score: 0; Stars, Snowflake, or Leaves 
- Exactness Stitch Width: 4 
- Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
- Tot Dig Score: 0]</t>
-  </si>
-  <si>
     <t>249</t>
   </si>
   <si>
@@ -1120,21 +1041,6 @@
     <t xml:space="preserve">260: [-2 SEPARATING SEMISEXTILE to MARS; 2 SEPARATING SEXTILE to JUPITER; -2 APPLYING SEMISQUARE to PLUTO] </t>
   </si>
   <si>
-    <t>260: [Snowflake 
- Exactness Stitch Width: 8 
- Aspect K/P:PatternStitchBase.PURL 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
- Tot Dig Score: 0; Stars, Snowflake, or Leaves 
- Exactness Stitch Width: 8 
- Aspect K/P:PatternStitchBase.PURL 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
- Tot Dig Score: 0; Chevron 
- Exactness Stitch Width: 8 
- Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
- Tot Dig Score: 0]</t>
-  </si>
-  <si>
     <t>261</t>
   </si>
   <si>
@@ -1171,17 +1077,6 @@
     <t xml:space="preserve">274: [-1 APPLYING BIQUINTILE to ASC; -3 APPLYING SEXTILE to PLUTO] </t>
   </si>
   <si>
-    <t>274: [ 
- Exactness Stitch Width: 9 
- Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
- Tot Dig Score: 0; Stars, Snowflake, or Leaves 
- Exactness Stitch Width: 7 
- Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
- Tot Dig Score: 0]</t>
-  </si>
-  <si>
     <t>276</t>
   </si>
   <si>
@@ -1224,29 +1119,6 @@
     <t xml:space="preserve">293: [7 APPLYING CONJ to SUN; 8 APPLYING CONJ to VENUS; 1 SEPARATING SEXTILE to MARS; -1 SEPARATING SEMISEXTILE to JUPITER; 1 SEPARATING SEMISQUARE to SATURN] </t>
   </si>
   <si>
-    <t>293: [Lines, circles, or Chains 
- Exactness Stitch Width: 3 
- Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
- Tot Dig Score: 4; Lines, circles, or Chains 
- Exactness Stitch Width: 2 
- Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
- Tot Dig Score: 0; Stars, Snowflake, or Leaves 
- Exactness Stitch Width: 9 
- Aspect K/P:PatternStitchBase.PURL 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
- Tot Dig Score: 0; Snowflake 
- Exactness Stitch Width: 9 
- Aspect K/P:PatternStitchBase.PURL 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
- Tot Dig Score: 0; Chevron 
- Exactness Stitch Width: 9 
- Aspect K/P:PatternStitchBase.PURL 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
- Tot Dig Score: 0]</t>
-  </si>
-  <si>
     <t>294</t>
   </si>
   <si>
@@ -1274,23 +1146,12 @@
     <t xml:space="preserve">300: [-4 SEPARATING TRINE to MOON; 7 APPLYING CONJ to MERCURY; 1 SEPARATING CONJ to VENUS; -7 APPLYING SQUARE to PLUTO] </t>
   </si>
   <si>
-    <t>300: [Diamonds, Triangles, or Leaves 
+    <t>300: [STITCH DETERMINER FOR: SEPARATING TRINE (SUN, MOON) [Score:Intensity: TRINE:8, Exactness:-4, Collective Planet Speed:17] 
+Diamonds, Triangles, or Leaves 
  Exactness Stitch Width: 6 
  Aspect K/P:PatternStitchBase.PURL 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
- Tot Dig Score: 5; Lines, circles, or Chains 
- Exactness Stitch Width: 3 
- Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
- Tot Dig Score: 4; Lines, circles, or Chains 
- Exactness Stitch Width: 9 
- Aspect K/P:PatternStitchBase.PURL 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
- Tot Dig Score: 4; Squares, or Diamonds 
- Exactness Stitch Width: 3 
- Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
- Tot Dig Score: 4]</t>
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [7, 10] 
+ Tot Dig Score: 5]</t>
   </si>
   <si>
     <t>303</t>
@@ -1339,17 +1200,6 @@
   </si>
   <si>
     <t xml:space="preserve">322: [-1 SEPARATING SEMISEXTILE to MERCURY; 2 SEPARATING SEXTILE to URANUS] </t>
-  </si>
-  <si>
-    <t>322: [Snowflake 
- Exactness Stitch Width: 9 
- Aspect K/P:PatternStitchBase.PURL 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
- Tot Dig Score: 0; Stars, Snowflake, or Leaves 
- Exactness Stitch Width: 8 
- Aspect K/P:PatternStitchBase.PURL 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [5, 3] 
- Tot Dig Score: 0]</t>
   </si>
   <si>
     <t>324</t>
@@ -3233,19 +3083,16 @@
       <c r="Q45" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="AF45" t="s">
-        <v>246</v>
-      </c>
       <c r="AG45">
         <v>44</v>
       </c>
     </row>
     <row r="46" spans="2:33">
       <c r="E46" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F46" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I46" s="8" t="s">
         <v>67</v>
@@ -3271,10 +3118,10 @@
     </row>
     <row r="47" spans="2:33">
       <c r="E47" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F47" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H47" s="3" t="s">
         <v>61</v>
@@ -3297,10 +3144,10 @@
     </row>
     <row r="48" spans="2:33">
       <c r="E48" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F48" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I48" s="8" t="s">
         <v>67</v>
@@ -3320,10 +3167,10 @@
     </row>
     <row r="49" spans="5:33">
       <c r="E49" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F49" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J49" s="9" t="s">
         <v>85</v>
@@ -3343,10 +3190,10 @@
     </row>
     <row r="50" spans="5:33">
       <c r="E50" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F50" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H50" s="3" t="s">
         <v>62</v>
@@ -3372,10 +3219,10 @@
     </row>
     <row r="51" spans="5:33">
       <c r="E51" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F51" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>55</v>
@@ -3407,10 +3254,10 @@
     </row>
     <row r="52" spans="5:33">
       <c r="E52" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F52" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>55</v>
@@ -3439,10 +3286,10 @@
     </row>
     <row r="53" spans="5:33">
       <c r="E53" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F53" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H53" s="3" t="s">
         <v>62</v>
@@ -3462,10 +3309,10 @@
     </row>
     <row r="54" spans="5:33">
       <c r="E54" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F54" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H54" s="3" t="s">
         <v>62</v>
@@ -3485,10 +3332,10 @@
     </row>
     <row r="55" spans="5:33">
       <c r="E55" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F55" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H55" s="3" t="s">
         <v>62</v>
@@ -3511,10 +3358,10 @@
     </row>
     <row r="56" spans="5:33">
       <c r="E56" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F56" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I56" s="8" t="s">
         <v>68</v>
@@ -3534,10 +3381,10 @@
     </row>
     <row r="57" spans="5:33">
       <c r="E57" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F57" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J57" s="9" t="s">
         <v>83</v>
@@ -3554,10 +3401,10 @@
     </row>
     <row r="58" spans="5:33">
       <c r="E58" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F58" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="J58" s="9" t="s">
         <v>83</v>
@@ -3577,10 +3424,10 @@
     </row>
     <row r="59" spans="5:33">
       <c r="E59" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F59" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>53</v>
@@ -3606,10 +3453,10 @@
     </row>
     <row r="60" spans="5:33">
       <c r="E60" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F60" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>53</v>
@@ -3641,10 +3488,10 @@
     </row>
     <row r="61" spans="5:33">
       <c r="E61" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F61" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>53</v>
@@ -3676,10 +3523,10 @@
     </row>
     <row r="62" spans="5:33">
       <c r="E62" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F62" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>53</v>
@@ -3705,10 +3552,10 @@
     </row>
     <row r="63" spans="5:33">
       <c r="E63" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F63" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>53</v>
@@ -3737,10 +3584,10 @@
     </row>
     <row r="64" spans="5:33">
       <c r="E64" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F64" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>53</v>
@@ -3769,10 +3616,10 @@
     </row>
     <row r="65" spans="2:33">
       <c r="E65" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F65" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H65" s="3" t="s">
         <v>63</v>
@@ -3792,10 +3639,10 @@
     </row>
     <row r="66" spans="2:33">
       <c r="E66" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F66" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I66" s="8" t="s">
         <v>69</v>
@@ -3815,10 +3662,10 @@
     </row>
     <row r="67" spans="2:33">
       <c r="E67" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F67" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I67" s="8" t="s">
         <v>69</v>
@@ -3838,10 +3685,10 @@
     </row>
     <row r="68" spans="2:33">
       <c r="E68" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F68" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J68" s="9" t="s">
         <v>82</v>
@@ -3861,10 +3708,10 @@
     </row>
     <row r="69" spans="2:33">
       <c r="E69" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F69" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>52</v>
@@ -3893,10 +3740,10 @@
     </row>
     <row r="70" spans="2:33">
       <c r="E70" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F70" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>52</v>
@@ -3919,10 +3766,10 @@
     </row>
     <row r="71" spans="2:33">
       <c r="E71" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F71" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>52</v>
@@ -3951,10 +3798,10 @@
     </row>
     <row r="72" spans="2:33">
       <c r="E72" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F72" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>52</v>
@@ -3980,10 +3827,10 @@
     </row>
     <row r="73" spans="2:33">
       <c r="E73" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F73" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G73" s="2" t="s">
         <v>52</v>
@@ -4012,16 +3859,16 @@
     </row>
     <row r="74" spans="2:33">
       <c r="B74" t="s">
+        <v>304</v>
+      </c>
+      <c r="D74" t="s">
         <v>305</v>
       </c>
-      <c r="D74" t="s">
-        <v>306</v>
-      </c>
       <c r="E74" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F74" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G74" s="2" t="s">
         <v>52</v>
@@ -4041,19 +3888,16 @@
       <c r="Q74" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="AF74" t="s">
-        <v>307</v>
-      </c>
       <c r="AG74">
         <v>73</v>
       </c>
     </row>
     <row r="75" spans="2:33">
       <c r="E75" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F75" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="I75" s="8" t="s">
         <v>72</v>
@@ -4070,10 +3914,10 @@
     </row>
     <row r="76" spans="2:33">
       <c r="E76" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F76" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="I76" s="8" t="s">
         <v>72</v>
@@ -4093,10 +3937,10 @@
     </row>
     <row r="77" spans="2:33">
       <c r="E77" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F77" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="I77" s="8" t="s">
         <v>72</v>
@@ -4119,10 +3963,10 @@
     </row>
     <row r="78" spans="2:33">
       <c r="E78" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F78" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="I78" s="8" t="s">
         <v>72</v>
@@ -4145,16 +3989,16 @@
     </row>
     <row r="79" spans="2:33">
       <c r="B79" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D79" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E79" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="F79" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="J79" s="9" t="s">
         <v>79</v>
@@ -4168,19 +4012,16 @@
       <c r="O79" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="AF79" t="s">
-        <v>320</v>
-      </c>
       <c r="AG79">
         <v>78</v>
       </c>
     </row>
     <row r="80" spans="2:33">
       <c r="E80" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="F80" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="G80" s="2" t="s">
         <v>49</v>
@@ -4206,10 +4047,10 @@
     </row>
     <row r="81" spans="2:33">
       <c r="E81" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="F81" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="G81" s="2" t="s">
         <v>49</v>
@@ -4238,10 +4079,10 @@
     </row>
     <row r="82" spans="2:33">
       <c r="E82" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="F82" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="G82" s="2" t="s">
         <v>49</v>
@@ -4267,10 +4108,10 @@
     </row>
     <row r="83" spans="2:33">
       <c r="E83" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F83" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>49</v>
@@ -4299,16 +4140,16 @@
     </row>
     <row r="84" spans="2:33">
       <c r="B84" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D84" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="E84" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="F84" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="H84" s="3" t="s">
         <v>66</v>
@@ -4325,19 +4166,16 @@
       <c r="Q84" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="AF84" t="s">
-        <v>333</v>
-      </c>
       <c r="AG84">
         <v>83</v>
       </c>
     </row>
     <row r="85" spans="2:33">
       <c r="E85" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="F85" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="H85" s="3" t="s">
         <v>66</v>
@@ -4357,10 +4195,10 @@
     </row>
     <row r="86" spans="2:33">
       <c r="E86" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="F86" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="H86" s="3" t="s">
         <v>66</v>
@@ -4380,10 +4218,10 @@
     </row>
     <row r="87" spans="2:33">
       <c r="E87" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F87" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="I87" s="8" t="s">
         <v>73</v>
@@ -4403,16 +4241,16 @@
     </row>
     <row r="88" spans="2:33">
       <c r="B88" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="D88" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="E88" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="F88" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="I88" s="8" t="s">
         <v>73</v>
@@ -4429,19 +4267,16 @@
       <c r="Q88" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="AF88" t="s">
-        <v>344</v>
-      </c>
       <c r="AG88">
         <v>87</v>
       </c>
     </row>
     <row r="89" spans="2:33">
       <c r="E89" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="F89" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="J89" s="9" t="s">
         <v>78</v>
@@ -4464,10 +4299,10 @@
     </row>
     <row r="90" spans="2:33">
       <c r="E90" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="F90" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="J90" s="9" t="s">
         <v>78</v>
@@ -4487,10 +4322,10 @@
     </row>
     <row r="91" spans="2:33">
       <c r="E91" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="F91" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="G91" s="2" t="s">
         <v>48</v>
@@ -4513,10 +4348,10 @@
     </row>
     <row r="92" spans="2:33">
       <c r="E92" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="F92" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="G92" s="2" t="s">
         <v>48</v>
@@ -4539,16 +4374,16 @@
     </row>
     <row r="93" spans="2:33">
       <c r="B93" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="D93" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="E93" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="F93" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="H93" s="3" t="s">
         <v>65</v>
@@ -4568,19 +4403,16 @@
       <c r="Q93" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="AF93" t="s">
-        <v>357</v>
-      </c>
       <c r="AG93">
         <v>92</v>
       </c>
     </row>
     <row r="94" spans="2:33">
       <c r="E94" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="F94" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="L94" s="12" t="s">
         <v>100</v>
@@ -4600,10 +4432,10 @@
     </row>
     <row r="95" spans="2:33">
       <c r="E95" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="F95" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="I95" s="8" t="s">
         <v>75</v>
@@ -4620,10 +4452,10 @@
     </row>
     <row r="96" spans="2:33">
       <c r="E96" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="F96" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="I96" s="8" t="s">
         <v>75</v>
@@ -4643,10 +4475,10 @@
     </row>
     <row r="97" spans="2:33">
       <c r="E97" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="F97" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="J97" s="9" t="s">
         <v>77</v>
@@ -4660,10 +4492,10 @@
     </row>
     <row r="98" spans="2:33">
       <c r="E98" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="F98" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="G98" s="2" t="s">
         <v>47</v>
@@ -4692,16 +4524,16 @@
     </row>
     <row r="99" spans="2:33">
       <c r="B99" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="D99" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="E99" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="F99" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="G99" s="2" t="s">
         <v>47</v>
@@ -4724,19 +4556,16 @@
       <c r="O99" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="AF99" t="s">
-        <v>372</v>
-      </c>
       <c r="AG99">
         <v>98</v>
       </c>
     </row>
     <row r="100" spans="2:33">
       <c r="E100" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="F100" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="G100" s="2" t="s">
         <v>47</v>
@@ -4759,10 +4588,10 @@
     </row>
     <row r="101" spans="2:33">
       <c r="E101" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="F101" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="G101" s="2" t="s">
         <v>47</v>
@@ -4788,19 +4617,19 @@
     </row>
     <row r="102" spans="2:33">
       <c r="B102" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="C102" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="D102" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="E102" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="F102" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="G102" s="2" t="s">
         <v>47</v>
@@ -4827,7 +4656,7 @@
         <v>152</v>
       </c>
       <c r="AF102" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="AG102">
         <v>101</v>
@@ -4835,10 +4664,10 @@
     </row>
     <row r="103" spans="2:33">
       <c r="E103" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="F103" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="G103" s="2" t="s">
         <v>47</v>
@@ -4873,10 +4702,10 @@
     </row>
     <row r="104" spans="2:33">
       <c r="E104" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="F104" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="G104" s="2" t="s">
         <v>47</v>
@@ -4905,10 +4734,10 @@
     </row>
     <row r="105" spans="2:33">
       <c r="E105" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="F105" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="G105" s="2" t="s">
         <v>47</v>
@@ -4934,10 +4763,10 @@
     </row>
     <row r="106" spans="2:33">
       <c r="E106" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="F106" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="I106" s="8" t="s">
         <v>76</v>
@@ -4963,10 +4792,10 @@
     </row>
     <row r="107" spans="2:33">
       <c r="E107" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="F107" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="I107" s="8" t="s">
         <v>76</v>
@@ -4989,10 +4818,10 @@
     </row>
     <row r="108" spans="2:33">
       <c r="E108" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="F108" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I108" s="8" t="s">
         <v>76</v>
@@ -5018,16 +4847,16 @@
     </row>
     <row r="109" spans="2:33">
       <c r="B109" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="D109" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="E109" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="F109" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="J109" s="9" t="s">
         <v>78</v>
@@ -5041,19 +4870,16 @@
       <c r="O109" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="AF109" t="s">
-        <v>399</v>
-      </c>
       <c r="AG109">
         <v>108</v>
       </c>
     </row>
     <row r="110" spans="2:33">
       <c r="E110" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="F110" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="H110" s="3" t="s">
         <v>62</v>
@@ -5076,10 +4902,10 @@
     </row>
     <row r="111" spans="2:33">
       <c r="E111" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="F111" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="G111" s="2" t="s">
         <v>48</v>
@@ -5111,10 +4937,10 @@
     </row>
     <row r="112" spans="2:33">
       <c r="E112" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="F112" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="G112" s="2" t="s">
         <v>48</v>
@@ -5146,10 +4972,10 @@
     </row>
     <row r="113" spans="5:33">
       <c r="E113" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="F113" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="H113" s="3" t="s">
         <v>62</v>
@@ -5169,10 +4995,10 @@
     </row>
     <row r="114" spans="5:33">
       <c r="E114" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="F114" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="H114" s="3" t="s">
         <v>62</v>
@@ -5195,10 +5021,10 @@
     </row>
     <row r="115" spans="5:33">
       <c r="E115" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="F115" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="H115" s="3" t="s">
         <v>62</v>
@@ -5224,10 +5050,10 @@
     </row>
     <row r="116" spans="5:33">
       <c r="E116" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="F116" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="G116" s="2" t="s">
         <v>50</v>
@@ -5256,10 +5082,10 @@
     </row>
     <row r="117" spans="5:33">
       <c r="E117" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="F117" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="G117" s="2" t="s">
         <v>50</v>
@@ -5285,10 +5111,10 @@
     </row>
     <row r="118" spans="5:33">
       <c r="E118" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="F118" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="J118" s="9" t="s">
         <v>79</v>
@@ -5308,10 +5134,10 @@
     </row>
     <row r="119" spans="5:33">
       <c r="E119" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="F119" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="J119" s="9" t="s">
         <v>79</v>
@@ -5331,10 +5157,10 @@
     </row>
     <row r="120" spans="5:33">
       <c r="E120" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="F120" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="G120" s="2" t="s">
         <v>49</v>
@@ -5360,10 +5186,10 @@
     </row>
     <row r="121" spans="5:33">
       <c r="E121" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="F121" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="G121" s="2" t="s">
         <v>49</v>

</xml_diff>